<commit_message>
Fix AAAA to match any local region of excel
</commit_message>
<xml_diff>
--- a/Listado Mis Comprobantes 2.0.xlsx
+++ b/Listado Mis Comprobantes 2.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\Descarga_MC_AFIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8090BF95-1CC3-41B5-92D7-C921734F0A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF0FC9F-DA7B-4A68-A94C-E8DDB7B44CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2216,7 +2216,8 @@
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="14.5703125" customWidth="1"/>
+    <col min="6" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
     <col min="10" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="16.5703125" customWidth="1"/>
     <col min="15" max="15" width="15" customWidth="1"/>
@@ -2322,11 +2323,11 @@
         <v>44895</v>
       </c>
       <c r="L2" s="2" t="str">
-        <f t="shared" ref="L2:L33" si="1">CONCATENATE(TEXT(A2,"0")," - ","MCE - ",TEXT(J2,"AAAAMM")," - ",SUBSTITUTE(D2,"-","")," - ",B2)</f>
+        <f>CONCATENATE(TEXT(A2,"0")," - ","MCE - ",YEAR(J2),TEXT(MONTH(J2),"00")," - ",SUBSTITUTE(D2,"-","")," - ",B2)</f>
         <v>0 - MCE - 202211 - 20000000000 - Cliente</v>
       </c>
       <c r="M2" s="2" t="str">
-        <f t="shared" ref="M2:M33" si="2">CONCATENATE(TEXT(A2,"0")," - ","MCR - ",TEXT(J2,"AAAAMM")," - ",SUBSTITUTE(D2,"-","")," - ",B2)</f>
+        <f>CONCATENATE(TEXT(A2,"0")," - ","MCR - ",YEAR(J2),TEXT(MONTH(J2),"00")," - ",SUBSTITUTE(D2,"-","")," - ",B2)</f>
         <v>0 - MCR - 202211 - 20000000000 - Cliente</v>
       </c>
       <c r="N2" s="5" t="str">
@@ -2338,27 +2339,27 @@
         <v>#N/A</v>
       </c>
       <c r="P2" s="5" t="e">
-        <f>IF(EXACT(O2,E2),"ü","x")</f>
+        <f t="shared" ref="P2:P33" si="1">IF(EXACT(O2,E2),"ü","x")</f>
         <v>#N/A</v>
       </c>
       <c r="Q2" s="4">
-        <f>ROW(A2)</f>
+        <f t="shared" ref="Q2:Q33" si="2">ROW(A2)</f>
         <v>2</v>
       </c>
-      <c r="R2" s="4" t="str">
-        <f>TEXT(J2,"AAAAMM")</f>
+      <c r="R2" s="2" t="str">
+        <f>YEAR(J2)&amp;TEXT(MONTH(J2),"00")</f>
         <v>202211</v>
       </c>
       <c r="S2" s="4">
-        <f>IF(C2=C1,1,0)</f>
+        <f t="shared" ref="S2:S33" si="3">IF(C2=C1,1,0)</f>
         <v>0</v>
       </c>
       <c r="T2" s="4">
-        <f>IF(C2=C3,1,0)</f>
+        <f t="shared" ref="T2:T33" si="4">IF(C2=C3,1,0)</f>
         <v>1</v>
       </c>
       <c r="U2" s="4">
-        <f t="shared" ref="U2:U33" si="3">SUM(S2:T2)</f>
+        <f t="shared" ref="U2:U33" si="5">SUM(S2:T2)</f>
         <v>1</v>
       </c>
     </row>
@@ -2387,19 +2388,19 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J66" si="4">F3</f>
+        <f t="shared" ref="J3:J66" si="6">F3</f>
         <v>44866</v>
       </c>
       <c r="K3" s="2">
-        <f t="shared" ref="K3:K66" si="5">EOMONTH(F3,0)</f>
+        <f t="shared" ref="K3:K66" si="7">EOMONTH(F3,0)</f>
         <v>44895</v>
       </c>
       <c r="L3" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="L3:L66" si="8">CONCATENATE(TEXT(A3,"0")," - ","MCE - ",YEAR(J3),TEXT(MONTH(J3),"00")," - ",SUBSTITUTE(D3,"-","")," - ",B3)</f>
         <v>0 - MCE - 202211 - 20000000000 - Cliente</v>
       </c>
       <c r="M3" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="M3:M66" si="9">CONCATENATE(TEXT(A3,"0")," - ","MCR - ",YEAR(J3),TEXT(MONTH(J3),"00")," - ",SUBSTITUTE(D3,"-","")," - ",B3)</f>
         <v>0 - MCR - 202211 - 20000000000 - Cliente</v>
       </c>
       <c r="N3" s="5" t="str">
@@ -2411,27 +2412,27 @@
         <v>#N/A</v>
       </c>
       <c r="P3" s="5" t="e">
-        <f>IF(EXACT(O3,E3),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q3" s="4">
-        <f>ROW(A3)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="R3" s="4" t="str">
-        <f>TEXT(J3,"AAAAMM")</f>
+      <c r="R3" s="2" t="str">
+        <f t="shared" ref="R3:R66" si="10">YEAR(J3)&amp;TEXT(MONTH(J3),"00")</f>
         <v>202211</v>
       </c>
       <c r="S3" s="4">
-        <f>IF(C3=C2,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T3" s="4">
-        <f>IF(C3=C4,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U3" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -2459,19 +2460,19 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L4" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M4" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N4" s="5" t="str">
@@ -2483,27 +2484,27 @@
         <v>#N/A</v>
       </c>
       <c r="P4" s="5" t="e">
-        <f>IF(EXACT(O4,E4),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q4" s="4">
-        <f>ROW(A4)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="R4" s="4" t="str">
-        <f>TEXT(J4,"AAAAMM")</f>
+      <c r="R4" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S4" s="4">
-        <f>IF(C4=C3,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T4" s="4">
-        <f>IF(C4=C5,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U4" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -2531,19 +2532,19 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K5" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L5" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M5" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N5" s="5" t="str">
@@ -2555,27 +2556,27 @@
         <v>#N/A</v>
       </c>
       <c r="P5" s="5" t="e">
-        <f>IF(EXACT(O5,E5),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q5" s="4">
-        <f>ROW(A5)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="R5" s="4" t="str">
-        <f>TEXT(J5,"AAAAMM")</f>
+      <c r="R5" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S5" s="4">
-        <f>IF(C5=C4,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T5" s="4">
-        <f>IF(C5=C6,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U5" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -2603,19 +2604,19 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L6" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M6" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N6" s="5" t="str">
@@ -2627,27 +2628,27 @@
         <v>#N/A</v>
       </c>
       <c r="P6" s="5" t="e">
-        <f>IF(EXACT(O6,E6),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q6" s="4">
-        <f>ROW(A6)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="R6" s="4" t="str">
-        <f>TEXT(J6,"AAAAMM")</f>
+      <c r="R6" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S6" s="4">
-        <f>IF(C6=C5,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T6" s="4">
-        <f>IF(C6=C7,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U6" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -2675,19 +2676,19 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L7" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M7" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N7" s="5" t="str">
@@ -2699,27 +2700,27 @@
         <v>#N/A</v>
       </c>
       <c r="P7" s="5" t="e">
-        <f>IF(EXACT(O7,E7),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q7" s="4">
-        <f>ROW(A7)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="R7" s="4" t="str">
-        <f>TEXT(J7,"AAAAMM")</f>
+      <c r="R7" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S7" s="4">
-        <f>IF(C7=C6,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T7" s="4">
-        <f>IF(C7=C8,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U7" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -2747,19 +2748,19 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K8" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L8" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M8" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N8" s="5" t="str">
@@ -2771,27 +2772,27 @@
         <v>#N/A</v>
       </c>
       <c r="P8" s="5" t="e">
-        <f>IF(EXACT(O8,E8),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q8" s="4">
-        <f>ROW(A8)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="R8" s="4" t="str">
-        <f>TEXT(J8,"AAAAMM")</f>
+      <c r="R8" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S8" s="4">
-        <f>IF(C8=C7,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T8" s="4">
-        <f>IF(C8=C9,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U8" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -2819,19 +2820,19 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K9" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L9" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M9" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N9" s="5" t="str">
@@ -2843,27 +2844,27 @@
         <v>#N/A</v>
       </c>
       <c r="P9" s="5" t="e">
-        <f>IF(EXACT(O9,E9),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q9" s="4">
-        <f>ROW(A9)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="R9" s="4" t="str">
-        <f>TEXT(J9,"AAAAMM")</f>
+      <c r="R9" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S9" s="4">
-        <f>IF(C9=C8,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T9" s="4">
-        <f>IF(C9=C10,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U9" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -2891,19 +2892,19 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K10" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L10" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M10" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N10" s="5" t="str">
@@ -2915,27 +2916,27 @@
         <v>#N/A</v>
       </c>
       <c r="P10" s="5" t="e">
-        <f>IF(EXACT(O10,E10),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q10" s="4">
-        <f>ROW(A10)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="R10" s="4" t="str">
-        <f>TEXT(J10,"AAAAMM")</f>
+      <c r="R10" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S10" s="4">
-        <f>IF(C10=C9,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T10" s="4">
-        <f>IF(C10=C11,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U10" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -2963,19 +2964,19 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K11" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L11" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M11" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N11" s="5" t="str">
@@ -2987,27 +2988,27 @@
         <v>#N/A</v>
       </c>
       <c r="P11" s="5" t="e">
-        <f>IF(EXACT(O11,E11),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q11" s="4">
-        <f>ROW(A11)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="R11" s="4" t="str">
-        <f>TEXT(J11,"AAAAMM")</f>
+      <c r="R11" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S11" s="4">
-        <f>IF(C11=C10,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T11" s="4">
-        <f>IF(C11=C12,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U11" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -3035,19 +3036,19 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K12" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L12" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M12" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N12" s="5" t="str">
@@ -3059,27 +3060,27 @@
         <v>#N/A</v>
       </c>
       <c r="P12" s="5" t="e">
-        <f>IF(EXACT(O12,E12),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q12" s="4">
-        <f>ROW(A12)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="R12" s="4" t="str">
-        <f>TEXT(J12,"AAAAMM")</f>
+      <c r="R12" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S12" s="4">
-        <f>IF(C12=C11,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T12" s="4">
-        <f>IF(C12=C13,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -3107,19 +3108,19 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L13" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M13" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N13" s="5" t="str">
@@ -3131,27 +3132,27 @@
         <v>#N/A</v>
       </c>
       <c r="P13" s="5" t="e">
-        <f>IF(EXACT(O13,E13),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q13" s="4">
-        <f>ROW(A13)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="R13" s="4" t="str">
-        <f>TEXT(J13,"AAAAMM")</f>
+      <c r="R13" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S13" s="4">
-        <f>IF(C13=C12,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T13" s="4">
-        <f>IF(C13=C14,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U13" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -3179,19 +3180,19 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K14" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L14" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M14" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N14" s="5" t="str">
@@ -3203,27 +3204,27 @@
         <v>#N/A</v>
       </c>
       <c r="P14" s="5" t="e">
-        <f>IF(EXACT(O14,E14),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q14" s="4">
-        <f>ROW(A14)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="R14" s="4" t="str">
-        <f>TEXT(J14,"AAAAMM")</f>
+      <c r="R14" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S14" s="4">
-        <f>IF(C14=C13,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T14" s="4">
-        <f>IF(C14=C15,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U14" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -3251,19 +3252,19 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K15" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L15" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M15" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N15" s="5" t="str">
@@ -3275,27 +3276,27 @@
         <v>#N/A</v>
       </c>
       <c r="P15" s="5" t="e">
-        <f>IF(EXACT(O15,E15),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q15" s="4">
-        <f>ROW(A15)</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="R15" s="4" t="str">
-        <f>TEXT(J15,"AAAAMM")</f>
+      <c r="R15" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S15" s="4">
-        <f>IF(C15=C14,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T15" s="4">
-        <f>IF(C15=C16,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U15" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -3323,19 +3324,19 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K16" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L16" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M16" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N16" s="5" t="str">
@@ -3347,27 +3348,27 @@
         <v>#N/A</v>
       </c>
       <c r="P16" s="5" t="e">
-        <f>IF(EXACT(O16,E16),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q16" s="4">
-        <f>ROW(A16)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="R16" s="4" t="str">
-        <f>TEXT(J16,"AAAAMM")</f>
+      <c r="R16" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S16" s="4">
-        <f>IF(C16=C15,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T16" s="4">
-        <f>IF(C16=C17,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U16" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -3395,19 +3396,19 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L17" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M17" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N17" s="5" t="str">
@@ -3419,27 +3420,27 @@
         <v>#N/A</v>
       </c>
       <c r="P17" s="5" t="e">
-        <f>IF(EXACT(O17,E17),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q17" s="4">
-        <f>ROW(A17)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="R17" s="4" t="str">
-        <f>TEXT(J17,"AAAAMM")</f>
+      <c r="R17" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S17" s="4">
-        <f>IF(C17=C16,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T17" s="4">
-        <f>IF(C17=C18,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U17" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -3467,19 +3468,19 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K18" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L18" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M18" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N18" s="5" t="str">
@@ -3491,27 +3492,27 @@
         <v>#N/A</v>
       </c>
       <c r="P18" s="5" t="e">
-        <f>IF(EXACT(O18,E18),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q18" s="4">
-        <f>ROW(A18)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="R18" s="4" t="str">
-        <f>TEXT(J18,"AAAAMM")</f>
+      <c r="R18" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S18" s="4">
-        <f>IF(C18=C17,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T18" s="4">
-        <f>IF(C18=C19,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U18" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -3539,19 +3540,19 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K19" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L19" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M19" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N19" s="5" t="str">
@@ -3563,27 +3564,27 @@
         <v>#N/A</v>
       </c>
       <c r="P19" s="5" t="e">
-        <f>IF(EXACT(O19,E19),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q19" s="4">
-        <f>ROW(A19)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="R19" s="4" t="str">
-        <f>TEXT(J19,"AAAAMM")</f>
+      <c r="R19" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S19" s="4">
-        <f>IF(C19=C18,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T19" s="4">
-        <f>IF(C19=C20,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U19" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -3611,19 +3612,19 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K20" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L20" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M20" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N20" s="5" t="str">
@@ -3635,27 +3636,27 @@
         <v>#N/A</v>
       </c>
       <c r="P20" s="5" t="e">
-        <f>IF(EXACT(O20,E20),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q20" s="4">
-        <f>ROW(A20)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="R20" s="4" t="str">
-        <f>TEXT(J20,"AAAAMM")</f>
+      <c r="R20" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S20" s="4">
-        <f>IF(C20=C19,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T20" s="4">
-        <f>IF(C20=C21,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U20" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -3683,19 +3684,19 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K21" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L21" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M21" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N21" s="5" t="str">
@@ -3707,27 +3708,27 @@
         <v>#N/A</v>
       </c>
       <c r="P21" s="5" t="e">
-        <f>IF(EXACT(O21,E21),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q21" s="4">
-        <f>ROW(A21)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="R21" s="4" t="str">
-        <f>TEXT(J21,"AAAAMM")</f>
+      <c r="R21" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S21" s="4">
-        <f>IF(C21=C20,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T21" s="4">
-        <f>IF(C21=C22,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U21" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -3755,19 +3756,19 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K22" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L22" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M22" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N22" s="5" t="str">
@@ -3779,27 +3780,27 @@
         <v>#N/A</v>
       </c>
       <c r="P22" s="5" t="e">
-        <f>IF(EXACT(O22,E22),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q22" s="4">
-        <f>ROW(A22)</f>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="R22" s="4" t="str">
-        <f>TEXT(J22,"AAAAMM")</f>
+      <c r="R22" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S22" s="4">
-        <f>IF(C22=C21,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T22" s="4">
-        <f>IF(C22=C23,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U22" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -3827,19 +3828,19 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K23" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L23" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M23" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N23" s="5" t="str">
@@ -3851,27 +3852,27 @@
         <v>#N/A</v>
       </c>
       <c r="P23" s="5" t="e">
-        <f>IF(EXACT(O23,E23),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q23" s="4">
-        <f>ROW(A23)</f>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="R23" s="4" t="str">
-        <f>TEXT(J23,"AAAAMM")</f>
+      <c r="R23" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S23" s="4">
-        <f>IF(C23=C22,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T23" s="4">
-        <f>IF(C23=C24,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U23" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -3899,19 +3900,19 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K24" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L24" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M24" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N24" s="5" t="str">
@@ -3923,27 +3924,27 @@
         <v>#N/A</v>
       </c>
       <c r="P24" s="5" t="e">
-        <f>IF(EXACT(O24,E24),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q24" s="4">
-        <f>ROW(A24)</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="R24" s="4" t="str">
-        <f>TEXT(J24,"AAAAMM")</f>
+      <c r="R24" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S24" s="4">
-        <f>IF(C24=C23,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T24" s="4">
-        <f>IF(C24=C25,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U24" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -3971,19 +3972,19 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K25" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L25" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M25" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N25" s="5" t="str">
@@ -3995,27 +3996,27 @@
         <v>#N/A</v>
       </c>
       <c r="P25" s="5" t="e">
-        <f>IF(EXACT(O25,E25),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q25" s="4">
-        <f>ROW(A25)</f>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="R25" s="4" t="str">
-        <f>TEXT(J25,"AAAAMM")</f>
+      <c r="R25" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S25" s="4">
-        <f>IF(C25=C24,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T25" s="4">
-        <f>IF(C25=C26,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U25" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -4043,19 +4044,19 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L26" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M26" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N26" s="5" t="str">
@@ -4067,27 +4068,27 @@
         <v>#N/A</v>
       </c>
       <c r="P26" s="5" t="e">
-        <f>IF(EXACT(O26,E26),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q26" s="4">
-        <f>ROW(A26)</f>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="R26" s="4" t="str">
-        <f>TEXT(J26,"AAAAMM")</f>
+      <c r="R26" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S26" s="4">
-        <f>IF(C26=C25,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T26" s="4">
-        <f>IF(C26=C27,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U26" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -4115,19 +4116,19 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K27" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L27" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M27" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N27" s="5" t="str">
@@ -4139,27 +4140,27 @@
         <v>#N/A</v>
       </c>
       <c r="P27" s="5" t="e">
-        <f>IF(EXACT(O27,E27),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q27" s="4">
-        <f>ROW(A27)</f>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="R27" s="4" t="str">
-        <f>TEXT(J27,"AAAAMM")</f>
+      <c r="R27" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S27" s="4">
-        <f>IF(C27=C26,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T27" s="4">
-        <f>IF(C27=C28,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U27" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -4187,19 +4188,19 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K28" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L28" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M28" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N28" s="5" t="str">
@@ -4211,27 +4212,27 @@
         <v>#N/A</v>
       </c>
       <c r="P28" s="5" t="e">
-        <f>IF(EXACT(O28,E28),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q28" s="4">
-        <f>ROW(A28)</f>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="R28" s="4" t="str">
-        <f>TEXT(J28,"AAAAMM")</f>
+      <c r="R28" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S28" s="4">
-        <f>IF(C28=C27,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T28" s="4">
-        <f>IF(C28=C29,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U28" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -4259,19 +4260,19 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K29" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L29" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M29" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N29" s="5" t="str">
@@ -4283,27 +4284,27 @@
         <v>#N/A</v>
       </c>
       <c r="P29" s="5" t="e">
-        <f>IF(EXACT(O29,E29),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q29" s="4">
-        <f>ROW(A29)</f>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="R29" s="4" t="str">
-        <f>TEXT(J29,"AAAAMM")</f>
+      <c r="R29" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S29" s="4">
-        <f>IF(C29=C28,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T29" s="4">
-        <f>IF(C29=C30,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U29" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -4331,19 +4332,19 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K30" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L30" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M30" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N30" s="5" t="str">
@@ -4355,27 +4356,27 @@
         <v>#N/A</v>
       </c>
       <c r="P30" s="5" t="e">
-        <f>IF(EXACT(O30,E30),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q30" s="4">
-        <f>ROW(A30)</f>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="R30" s="4" t="str">
-        <f>TEXT(J30,"AAAAMM")</f>
+      <c r="R30" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S30" s="4">
-        <f>IF(C30=C29,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T30" s="4">
-        <f>IF(C30=C31,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U30" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -4403,19 +4404,19 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K31" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L31" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M31" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N31" s="5" t="str">
@@ -4427,27 +4428,27 @@
         <v>#N/A</v>
       </c>
       <c r="P31" s="5" t="e">
-        <f>IF(EXACT(O31,E31),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q31" s="4">
-        <f>ROW(A31)</f>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="R31" s="4" t="str">
-        <f>TEXT(J31,"AAAAMM")</f>
+      <c r="R31" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S31" s="4">
-        <f>IF(C31=C30,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T31" s="4">
-        <f>IF(C31=C32,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U31" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -4475,19 +4476,19 @@
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K32" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L32" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M32" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N32" s="5" t="str">
@@ -4499,27 +4500,27 @@
         <v>#N/A</v>
       </c>
       <c r="P32" s="5" t="e">
-        <f>IF(EXACT(O32,E32),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q32" s="4">
-        <f>ROW(A32)</f>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="R32" s="4" t="str">
-        <f>TEXT(J32,"AAAAMM")</f>
+      <c r="R32" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S32" s="4">
-        <f>IF(C32=C31,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T32" s="4">
-        <f>IF(C32=C33,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U32" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -4547,19 +4548,19 @@
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K33" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L33" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M33" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N33" s="5" t="str">
@@ -4571,33 +4572,33 @@
         <v>#N/A</v>
       </c>
       <c r="P33" s="5" t="e">
-        <f>IF(EXACT(O33,E33),"ü","x")</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q33" s="4">
-        <f>ROW(A33)</f>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="R33" s="4" t="str">
-        <f>TEXT(J33,"AAAAMM")</f>
+      <c r="R33" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S33" s="4">
-        <f>IF(C33=C32,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T33" s="4">
-        <f>IF(C33=C34,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U33" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="str">
-        <f t="shared" ref="A34:A69" si="6">RIGHT(D34,1)</f>
+        <f t="shared" ref="A34:A69" si="11">RIGHT(D34,1)</f>
         <v>0</v>
       </c>
       <c r="B34" t="s">
@@ -4619,19 +4620,19 @@
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="J34" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K34" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L34" s="2" t="str">
-        <f t="shared" ref="L34:L69" si="7">CONCATENATE(TEXT(A34,"0")," - ","MCE - ",TEXT(J34,"AAAAMM")," - ",SUBSTITUTE(D34,"-","")," - ",B34)</f>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M34" s="2" t="str">
-        <f t="shared" ref="M34:M69" si="8">CONCATENATE(TEXT(A34,"0")," - ","MCR - ",TEXT(J34,"AAAAMM")," - ",SUBSTITUTE(D34,"-","")," - ",B34)</f>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N34" s="5" t="str">
@@ -4643,33 +4644,33 @@
         <v>#N/A</v>
       </c>
       <c r="P34" s="5" t="e">
-        <f>IF(EXACT(O34,E34),"ü","x")</f>
+        <f t="shared" ref="P34:P65" si="12">IF(EXACT(O34,E34),"ü","x")</f>
         <v>#N/A</v>
       </c>
       <c r="Q34" s="4">
-        <f>ROW(A34)</f>
+        <f t="shared" ref="Q34:Q69" si="13">ROW(A34)</f>
         <v>34</v>
       </c>
-      <c r="R34" s="4" t="str">
-        <f>TEXT(J34,"AAAAMM")</f>
+      <c r="R34" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S34" s="4">
-        <f>IF(C34=C33,1,0)</f>
+        <f t="shared" ref="S34:S67" si="14">IF(C34=C33,1,0)</f>
         <v>1</v>
       </c>
       <c r="T34" s="4">
-        <f>IF(C34=C35,1,0)</f>
+        <f t="shared" ref="T34:T67" si="15">IF(C34=C35,1,0)</f>
         <v>1</v>
       </c>
       <c r="U34" s="4">
-        <f t="shared" ref="U34:U65" si="9">SUM(S34:T34)</f>
+        <f t="shared" ref="U34:U65" si="16">SUM(S34:T34)</f>
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B35" t="s">
@@ -4691,19 +4692,19 @@
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
       <c r="J35" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K35" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L35" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M35" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N35" s="5" t="str">
@@ -4715,33 +4716,33 @@
         <v>#N/A</v>
       </c>
       <c r="P35" s="5" t="e">
-        <f>IF(EXACT(O35,E35),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q35" s="4">
-        <f>ROW(A35)</f>
+        <f t="shared" si="13"/>
         <v>35</v>
       </c>
-      <c r="R35" s="4" t="str">
-        <f>TEXT(J35,"AAAAMM")</f>
+      <c r="R35" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S35" s="4">
-        <f>IF(C35=C34,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T35" s="4">
-        <f>IF(C35=C36,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U35" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B36" t="s">
@@ -4763,19 +4764,19 @@
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="J36" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K36" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L36" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M36" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N36" s="5" t="str">
@@ -4787,33 +4788,33 @@
         <v>#N/A</v>
       </c>
       <c r="P36" s="5" t="e">
-        <f>IF(EXACT(O36,E36),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q36" s="4">
-        <f>ROW(A36)</f>
+        <f t="shared" si="13"/>
         <v>36</v>
       </c>
-      <c r="R36" s="4" t="str">
-        <f>TEXT(J36,"AAAAMM")</f>
+      <c r="R36" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S36" s="4">
-        <f>IF(C36=C35,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T36" s="4">
-        <f>IF(C36=C37,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U36" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B37" t="s">
@@ -4835,19 +4836,19 @@
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="J37" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K37" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L37" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M37" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N37" s="5" t="str">
@@ -4859,33 +4860,33 @@
         <v>#N/A</v>
       </c>
       <c r="P37" s="5" t="e">
-        <f>IF(EXACT(O37,E37),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q37" s="4">
-        <f>ROW(A37)</f>
+        <f t="shared" si="13"/>
         <v>37</v>
       </c>
-      <c r="R37" s="4" t="str">
-        <f>TEXT(J37,"AAAAMM")</f>
+      <c r="R37" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S37" s="4">
-        <f>IF(C37=C36,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T37" s="4">
-        <f>IF(C37=C38,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U37" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B38" t="s">
@@ -4907,19 +4908,19 @@
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
       <c r="J38" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K38" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L38" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M38" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N38" s="5" t="str">
@@ -4931,33 +4932,33 @@
         <v>#N/A</v>
       </c>
       <c r="P38" s="5" t="e">
-        <f>IF(EXACT(O38,E38),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q38" s="4">
-        <f>ROW(A38)</f>
+        <f t="shared" si="13"/>
         <v>38</v>
       </c>
-      <c r="R38" s="4" t="str">
-        <f>TEXT(J38,"AAAAMM")</f>
+      <c r="R38" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S38" s="4">
-        <f>IF(C38=C37,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T38" s="4">
-        <f>IF(C38=C39,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U38" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B39" t="s">
@@ -4979,19 +4980,19 @@
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
       <c r="J39" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L39" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M39" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N39" s="5" t="str">
@@ -5003,33 +5004,33 @@
         <v>#N/A</v>
       </c>
       <c r="P39" s="5" t="e">
-        <f>IF(EXACT(O39,E39),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q39" s="4">
-        <f>ROW(A39)</f>
+        <f t="shared" si="13"/>
         <v>39</v>
       </c>
-      <c r="R39" s="4" t="str">
-        <f>TEXT(J39,"AAAAMM")</f>
+      <c r="R39" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S39" s="4">
-        <f>IF(C39=C38,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T39" s="4">
-        <f>IF(C39=C40,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U39" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B40" t="s">
@@ -5051,19 +5052,19 @@
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
       <c r="J40" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K40" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L40" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M40" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N40" s="5" t="str">
@@ -5075,33 +5076,33 @@
         <v>#N/A</v>
       </c>
       <c r="P40" s="5" t="e">
-        <f>IF(EXACT(O40,E40),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q40" s="4">
-        <f>ROW(A40)</f>
+        <f t="shared" si="13"/>
         <v>40</v>
       </c>
-      <c r="R40" s="4" t="str">
-        <f>TEXT(J40,"AAAAMM")</f>
+      <c r="R40" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S40" s="4">
-        <f>IF(C40=C39,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T40" s="4">
-        <f>IF(C40=C41,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U40" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B41" t="s">
@@ -5123,19 +5124,19 @@
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
       <c r="J41" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K41" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L41" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M41" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N41" s="5" t="str">
@@ -5147,33 +5148,33 @@
         <v>#N/A</v>
       </c>
       <c r="P41" s="5" t="e">
-        <f>IF(EXACT(O41,E41),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q41" s="4">
-        <f>ROW(A41)</f>
+        <f t="shared" si="13"/>
         <v>41</v>
       </c>
-      <c r="R41" s="4" t="str">
-        <f>TEXT(J41,"AAAAMM")</f>
+      <c r="R41" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S41" s="4">
-        <f>IF(C41=C40,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T41" s="4">
-        <f>IF(C41=C42,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U41" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B42" t="s">
@@ -5195,19 +5196,19 @@
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
       <c r="J42" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K42" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L42" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M42" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N42" s="5" t="str">
@@ -5219,33 +5220,33 @@
         <v>#N/A</v>
       </c>
       <c r="P42" s="5" t="e">
-        <f>IF(EXACT(O42,E42),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q42" s="4">
-        <f>ROW(A42)</f>
+        <f t="shared" si="13"/>
         <v>42</v>
       </c>
-      <c r="R42" s="4" t="str">
-        <f>TEXT(J42,"AAAAMM")</f>
+      <c r="R42" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S42" s="4">
-        <f>IF(C42=C41,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T42" s="4">
-        <f>IF(C42=C43,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U42" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B43" t="s">
@@ -5267,19 +5268,19 @@
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K43" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L43" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M43" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N43" s="5" t="str">
@@ -5291,33 +5292,33 @@
         <v>#N/A</v>
       </c>
       <c r="P43" s="5" t="e">
-        <f>IF(EXACT(O43,E43),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q43" s="4">
-        <f>ROW(A43)</f>
+        <f t="shared" si="13"/>
         <v>43</v>
       </c>
-      <c r="R43" s="4" t="str">
-        <f>TEXT(J43,"AAAAMM")</f>
+      <c r="R43" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S43" s="4">
-        <f>IF(C43=C42,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T43" s="4">
-        <f>IF(C43=C44,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U43" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B44" t="s">
@@ -5339,19 +5340,19 @@
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
       <c r="J44" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K44" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L44" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M44" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N44" s="5" t="str">
@@ -5363,33 +5364,33 @@
         <v>#N/A</v>
       </c>
       <c r="P44" s="5" t="e">
-        <f>IF(EXACT(O44,E44),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q44" s="4">
-        <f>ROW(A44)</f>
+        <f t="shared" si="13"/>
         <v>44</v>
       </c>
-      <c r="R44" s="4" t="str">
-        <f>TEXT(J44,"AAAAMM")</f>
+      <c r="R44" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S44" s="4">
-        <f>IF(C44=C43,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T44" s="4">
-        <f>IF(C44=C45,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U44" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B45" t="s">
@@ -5411,19 +5412,19 @@
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
       <c r="J45" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K45" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L45" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M45" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N45" s="5" t="str">
@@ -5435,33 +5436,33 @@
         <v>#N/A</v>
       </c>
       <c r="P45" s="5" t="e">
-        <f>IF(EXACT(O45,E45),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q45" s="4">
-        <f>ROW(A45)</f>
+        <f t="shared" si="13"/>
         <v>45</v>
       </c>
-      <c r="R45" s="4" t="str">
-        <f>TEXT(J45,"AAAAMM")</f>
+      <c r="R45" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S45" s="4">
-        <f>IF(C45=C44,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T45" s="4">
-        <f>IF(C45=C46,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U45" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B46" t="s">
@@ -5483,19 +5484,19 @@
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="J46" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K46" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L46" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M46" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N46" s="5" t="str">
@@ -5507,33 +5508,33 @@
         <v>#N/A</v>
       </c>
       <c r="P46" s="5" t="e">
-        <f>IF(EXACT(O46,E46),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q46" s="4">
-        <f>ROW(A46)</f>
+        <f t="shared" si="13"/>
         <v>46</v>
       </c>
-      <c r="R46" s="4" t="str">
-        <f>TEXT(J46,"AAAAMM")</f>
+      <c r="R46" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S46" s="4">
-        <f>IF(C46=C45,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T46" s="4">
-        <f>IF(C46=C47,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U46" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B47" t="s">
@@ -5555,19 +5556,19 @@
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
       <c r="J47" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K47" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L47" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M47" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N47" s="5" t="str">
@@ -5579,33 +5580,33 @@
         <v>#N/A</v>
       </c>
       <c r="P47" s="5" t="e">
-        <f>IF(EXACT(O47,E47),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q47" s="4">
-        <f>ROW(A47)</f>
+        <f t="shared" si="13"/>
         <v>47</v>
       </c>
-      <c r="R47" s="4" t="str">
-        <f>TEXT(J47,"AAAAMM")</f>
+      <c r="R47" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S47" s="4">
-        <f>IF(C47=C46,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T47" s="4">
-        <f>IF(C47=C48,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U47" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B48" t="s">
@@ -5627,19 +5628,19 @@
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
       <c r="J48" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K48" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L48" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M48" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N48" s="5" t="str">
@@ -5651,33 +5652,33 @@
         <v>#N/A</v>
       </c>
       <c r="P48" s="5" t="e">
-        <f>IF(EXACT(O48,E48),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q48" s="4">
-        <f>ROW(A48)</f>
+        <f t="shared" si="13"/>
         <v>48</v>
       </c>
-      <c r="R48" s="4" t="str">
-        <f>TEXT(J48,"AAAAMM")</f>
+      <c r="R48" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S48" s="4">
-        <f>IF(C48=C47,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T48" s="4">
-        <f>IF(C48=C49,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U48" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B49" t="s">
@@ -5699,19 +5700,19 @@
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
       <c r="J49" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K49" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L49" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M49" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N49" s="5" t="str">
@@ -5723,33 +5724,33 @@
         <v>#N/A</v>
       </c>
       <c r="P49" s="5" t="e">
-        <f>IF(EXACT(O49,E49),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q49" s="4">
-        <f>ROW(A49)</f>
+        <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="R49" s="4" t="str">
-        <f>TEXT(J49,"AAAAMM")</f>
+      <c r="R49" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S49" s="4">
-        <f>IF(C49=C48,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T49" s="4">
-        <f>IF(C49=C50,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U49" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B50" t="s">
@@ -5771,19 +5772,19 @@
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
       <c r="J50" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K50" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L50" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M50" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N50" s="5" t="str">
@@ -5795,33 +5796,33 @@
         <v>#N/A</v>
       </c>
       <c r="P50" s="5" t="e">
-        <f>IF(EXACT(O50,E50),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q50" s="4">
-        <f>ROW(A50)</f>
+        <f t="shared" si="13"/>
         <v>50</v>
       </c>
-      <c r="R50" s="4" t="str">
-        <f>TEXT(J50,"AAAAMM")</f>
+      <c r="R50" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S50" s="4">
-        <f>IF(C50=C49,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T50" s="4">
-        <f>IF(C50=C51,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U50" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B51" t="s">
@@ -5843,19 +5844,19 @@
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
       <c r="J51" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K51" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L51" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M51" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N51" s="5" t="str">
@@ -5867,33 +5868,33 @@
         <v>#N/A</v>
       </c>
       <c r="P51" s="5" t="e">
-        <f>IF(EXACT(O51,E51),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q51" s="4">
-        <f>ROW(A51)</f>
+        <f t="shared" si="13"/>
         <v>51</v>
       </c>
-      <c r="R51" s="4" t="str">
-        <f>TEXT(J51,"AAAAMM")</f>
+      <c r="R51" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S51" s="4">
-        <f>IF(C51=C50,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T51" s="4">
-        <f>IF(C51=C52,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U51" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B52" t="s">
@@ -5915,19 +5916,19 @@
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
       <c r="J52" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K52" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L52" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M52" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N52" s="5" t="str">
@@ -5939,33 +5940,33 @@
         <v>#N/A</v>
       </c>
       <c r="P52" s="5" t="e">
-        <f>IF(EXACT(O52,E52),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q52" s="4">
-        <f>ROW(A52)</f>
+        <f t="shared" si="13"/>
         <v>52</v>
       </c>
-      <c r="R52" s="4" t="str">
-        <f>TEXT(J52,"AAAAMM")</f>
+      <c r="R52" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S52" s="4">
-        <f>IF(C52=C51,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T52" s="4">
-        <f>IF(C52=C53,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U52" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B53" t="s">
@@ -5987,19 +5988,19 @@
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
       <c r="J53" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K53" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L53" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M53" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N53" s="5" t="str">
@@ -6011,33 +6012,33 @@
         <v>#N/A</v>
       </c>
       <c r="P53" s="5" t="e">
-        <f>IF(EXACT(O53,E53),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q53" s="4">
-        <f>ROW(A53)</f>
+        <f t="shared" si="13"/>
         <v>53</v>
       </c>
-      <c r="R53" s="4" t="str">
-        <f>TEXT(J53,"AAAAMM")</f>
+      <c r="R53" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S53" s="4">
-        <f>IF(C53=C52,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T53" s="4">
-        <f>IF(C53=C54,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U53" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B54" t="s">
@@ -6059,19 +6060,19 @@
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K54" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L54" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M54" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N54" s="5" t="str">
@@ -6083,33 +6084,33 @@
         <v>#N/A</v>
       </c>
       <c r="P54" s="5" t="e">
-        <f>IF(EXACT(O54,E54),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q54" s="4">
-        <f>ROW(A54)</f>
+        <f t="shared" si="13"/>
         <v>54</v>
       </c>
-      <c r="R54" s="4" t="str">
-        <f>TEXT(J54,"AAAAMM")</f>
+      <c r="R54" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S54" s="4">
-        <f>IF(C54=C53,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T54" s="4">
-        <f>IF(C54=C55,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U54" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B55" t="s">
@@ -6131,19 +6132,19 @@
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
       <c r="J55" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K55" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L55" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M55" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N55" s="5" t="str">
@@ -6155,33 +6156,33 @@
         <v>#N/A</v>
       </c>
       <c r="P55" s="5" t="e">
-        <f>IF(EXACT(O55,E55),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q55" s="4">
-        <f>ROW(A55)</f>
+        <f t="shared" si="13"/>
         <v>55</v>
       </c>
-      <c r="R55" s="4" t="str">
-        <f>TEXT(J55,"AAAAMM")</f>
+      <c r="R55" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S55" s="4">
-        <f>IF(C55=C54,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T55" s="4">
-        <f>IF(C55=C56,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U55" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B56" t="s">
@@ -6203,19 +6204,19 @@
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
       <c r="J56" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K56" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L56" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M56" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N56" s="5" t="str">
@@ -6227,33 +6228,33 @@
         <v>#N/A</v>
       </c>
       <c r="P56" s="5" t="e">
-        <f>IF(EXACT(O56,E56),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q56" s="4">
-        <f>ROW(A56)</f>
+        <f t="shared" si="13"/>
         <v>56</v>
       </c>
-      <c r="R56" s="4" t="str">
-        <f>TEXT(J56,"AAAAMM")</f>
+      <c r="R56" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S56" s="4">
-        <f>IF(C56=C55,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T56" s="4">
-        <f>IF(C56=C57,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U56" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B57" t="s">
@@ -6275,19 +6276,19 @@
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
       <c r="J57" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K57" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L57" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M57" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N57" s="5" t="str">
@@ -6299,33 +6300,33 @@
         <v>#N/A</v>
       </c>
       <c r="P57" s="5" t="e">
-        <f>IF(EXACT(O57,E57),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q57" s="4">
-        <f>ROW(A57)</f>
+        <f t="shared" si="13"/>
         <v>57</v>
       </c>
-      <c r="R57" s="4" t="str">
-        <f>TEXT(J57,"AAAAMM")</f>
+      <c r="R57" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S57" s="4">
-        <f>IF(C57=C56,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T57" s="4">
-        <f>IF(C57=C58,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U57" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B58" t="s">
@@ -6347,19 +6348,19 @@
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
       <c r="J58" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K58" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L58" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M58" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N58" s="5" t="str">
@@ -6371,33 +6372,33 @@
         <v>#N/A</v>
       </c>
       <c r="P58" s="5" t="e">
-        <f>IF(EXACT(O58,E58),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q58" s="4">
-        <f>ROW(A58)</f>
+        <f t="shared" si="13"/>
         <v>58</v>
       </c>
-      <c r="R58" s="4" t="str">
-        <f>TEXT(J58,"AAAAMM")</f>
+      <c r="R58" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S58" s="4">
-        <f>IF(C58=C57,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T58" s="4">
-        <f>IF(C58=C59,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U58" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B59" t="s">
@@ -6419,19 +6420,19 @@
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
       <c r="J59" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K59" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L59" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M59" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N59" s="5" t="str">
@@ -6443,33 +6444,33 @@
         <v>#N/A</v>
       </c>
       <c r="P59" s="5" t="e">
-        <f>IF(EXACT(O59,E59),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q59" s="4">
-        <f>ROW(A59)</f>
+        <f t="shared" si="13"/>
         <v>59</v>
       </c>
-      <c r="R59" s="4" t="str">
-        <f>TEXT(J59,"AAAAMM")</f>
+      <c r="R59" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S59" s="4">
-        <f>IF(C59=C58,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T59" s="4">
-        <f>IF(C59=C60,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U59" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B60" t="s">
@@ -6491,19 +6492,19 @@
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
       <c r="J60" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K60" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L60" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M60" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N60" s="5" t="str">
@@ -6515,33 +6516,33 @@
         <v>#N/A</v>
       </c>
       <c r="P60" s="5" t="e">
-        <f>IF(EXACT(O60,E60),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q60" s="4">
-        <f>ROW(A60)</f>
+        <f t="shared" si="13"/>
         <v>60</v>
       </c>
-      <c r="R60" s="4" t="str">
-        <f>TEXT(J60,"AAAAMM")</f>
+      <c r="R60" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S60" s="4">
-        <f>IF(C60=C59,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T60" s="4">
-        <f>IF(C60=C61,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U60" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B61" t="s">
@@ -6563,19 +6564,19 @@
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
       <c r="J61" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K61" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L61" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M61" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N61" s="5" t="str">
@@ -6587,33 +6588,33 @@
         <v>#N/A</v>
       </c>
       <c r="P61" s="5" t="e">
-        <f>IF(EXACT(O61,E61),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q61" s="4">
-        <f>ROW(A61)</f>
+        <f t="shared" si="13"/>
         <v>61</v>
       </c>
-      <c r="R61" s="4" t="str">
-        <f>TEXT(J61,"AAAAMM")</f>
+      <c r="R61" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S61" s="4">
-        <f>IF(C61=C60,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T61" s="4">
-        <f>IF(C61=C62,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U61" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B62" t="s">
@@ -6635,19 +6636,19 @@
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
       <c r="J62" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K62" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L62" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M62" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N62" s="5" t="str">
@@ -6659,33 +6660,33 @@
         <v>#N/A</v>
       </c>
       <c r="P62" s="5" t="e">
-        <f>IF(EXACT(O62,E62),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q62" s="4">
-        <f>ROW(A62)</f>
+        <f t="shared" si="13"/>
         <v>62</v>
       </c>
-      <c r="R62" s="4" t="str">
-        <f>TEXT(J62,"AAAAMM")</f>
+      <c r="R62" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S62" s="4">
-        <f>IF(C62=C61,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T62" s="4">
-        <f>IF(C62=C63,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U62" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B63" t="s">
@@ -6707,19 +6708,19 @@
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
       <c r="J63" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K63" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L63" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M63" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N63" s="5" t="str">
@@ -6731,33 +6732,33 @@
         <v>#N/A</v>
       </c>
       <c r="P63" s="5" t="e">
-        <f>IF(EXACT(O63,E63),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q63" s="4">
-        <f>ROW(A63)</f>
+        <f t="shared" si="13"/>
         <v>63</v>
       </c>
-      <c r="R63" s="4" t="str">
-        <f>TEXT(J63,"AAAAMM")</f>
+      <c r="R63" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S63" s="4">
-        <f>IF(C63=C62,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T63" s="4">
-        <f>IF(C63=C64,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U63" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B64" t="s">
@@ -6779,19 +6780,19 @@
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
       <c r="J64" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K64" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L64" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M64" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N64" s="5" t="str">
@@ -6803,33 +6804,33 @@
         <v>#N/A</v>
       </c>
       <c r="P64" s="5" t="e">
-        <f>IF(EXACT(O64,E64),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q64" s="4">
-        <f>ROW(A64)</f>
+        <f t="shared" si="13"/>
         <v>64</v>
       </c>
-      <c r="R64" s="4" t="str">
-        <f>TEXT(J64,"AAAAMM")</f>
+      <c r="R64" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S64" s="4">
-        <f>IF(C64=C63,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T64" s="4">
-        <f>IF(C64=C65,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U64" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B65" t="s">
@@ -6851,19 +6852,19 @@
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
       <c r="J65" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K65" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L65" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M65" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N65" s="5" t="str">
@@ -6875,33 +6876,33 @@
         <v>#N/A</v>
       </c>
       <c r="P65" s="5" t="e">
-        <f>IF(EXACT(O65,E65),"ü","x")</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="Q65" s="4">
-        <f>ROW(A65)</f>
+        <f t="shared" si="13"/>
         <v>65</v>
       </c>
-      <c r="R65" s="4" t="str">
-        <f>TEXT(J65,"AAAAMM")</f>
+      <c r="R65" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S65" s="4">
-        <f>IF(C65=C64,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T65" s="4">
-        <f>IF(C65=C66,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U65" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B66" t="s">
@@ -6923,19 +6924,19 @@
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
       <c r="J66" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44866</v>
       </c>
       <c r="K66" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44895</v>
       </c>
       <c r="L66" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M66" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N66" s="5" t="str">
@@ -6947,33 +6948,33 @@
         <v>#N/A</v>
       </c>
       <c r="P66" s="5" t="e">
-        <f>IF(EXACT(O66,E66),"ü","x")</f>
+        <f t="shared" ref="P66:P97" si="17">IF(EXACT(O66,E66),"ü","x")</f>
         <v>#N/A</v>
       </c>
       <c r="Q66" s="4">
-        <f>ROW(A66)</f>
+        <f t="shared" si="13"/>
         <v>66</v>
       </c>
-      <c r="R66" s="4" t="str">
-        <f>TEXT(J66,"AAAAMM")</f>
+      <c r="R66" s="2" t="str">
+        <f t="shared" si="10"/>
         <v>202211</v>
       </c>
       <c r="S66" s="4">
-        <f>IF(C66=C65,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T66" s="4">
-        <f>IF(C66=C67,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U66" s="4">
-        <f t="shared" ref="U66:U69" si="10">SUM(S66:T66)</f>
+        <f t="shared" ref="U66:U69" si="18">SUM(S66:T66)</f>
         <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B67" t="s">
@@ -6995,19 +6996,19 @@
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
       <c r="J67" s="2">
-        <f t="shared" ref="J67:J69" si="11">F67</f>
+        <f t="shared" ref="J67:J69" si="19">F67</f>
         <v>44866</v>
       </c>
       <c r="K67" s="2">
-        <f t="shared" ref="K67:K69" si="12">EOMONTH(F67,0)</f>
+        <f t="shared" ref="K67:K69" si="20">EOMONTH(F67,0)</f>
         <v>44895</v>
       </c>
       <c r="L67" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="L67:L69" si="21">CONCATENATE(TEXT(A67,"0")," - ","MCE - ",YEAR(J67),TEXT(MONTH(J67),"00")," - ",SUBSTITUTE(D67,"-","")," - ",B67)</f>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M67" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="M67:M69" si="22">CONCATENATE(TEXT(A67,"0")," - ","MCR - ",YEAR(J67),TEXT(MONTH(J67),"00")," - ",SUBSTITUTE(D67,"-","")," - ",B67)</f>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N67" s="5" t="str">
@@ -7019,33 +7020,33 @@
         <v>#N/A</v>
       </c>
       <c r="P67" s="5" t="e">
-        <f>IF(EXACT(O67,E67),"ü","x")</f>
+        <f t="shared" si="17"/>
         <v>#N/A</v>
       </c>
       <c r="Q67" s="4">
-        <f>ROW(A67)</f>
+        <f t="shared" si="13"/>
         <v>67</v>
       </c>
-      <c r="R67" s="4" t="str">
-        <f>TEXT(J67,"AAAAMM")</f>
+      <c r="R67" s="2" t="str">
+        <f t="shared" ref="R67:R69" si="23">YEAR(J67)&amp;TEXT(MONTH(J67),"00")</f>
         <v>202211</v>
       </c>
       <c r="S67" s="4">
-        <f>IF(C67=C66,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T67" s="4">
-        <f>IF(C67=C68,1,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U67" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B68" t="s">
@@ -7067,19 +7068,19 @@
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
       <c r="J68" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>44866</v>
       </c>
       <c r="K68" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>44895</v>
       </c>
       <c r="L68" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="21"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M68" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N68" s="5" t="str">
@@ -7091,33 +7092,33 @@
         <v>#N/A</v>
       </c>
       <c r="P68" s="5" t="e">
-        <f>IF(EXACT(O68,E68),"ü","x")</f>
+        <f t="shared" si="17"/>
         <v>#N/A</v>
       </c>
       <c r="Q68" s="4">
-        <f>ROW(A68)</f>
+        <f t="shared" si="13"/>
         <v>68</v>
       </c>
-      <c r="R68" s="4" t="str">
-        <f>TEXT(J68,"AAAAMM")</f>
+      <c r="R68" s="2" t="str">
+        <f t="shared" si="23"/>
         <v>202211</v>
       </c>
       <c r="S68" s="4">
-        <f t="shared" ref="S68:S69" si="13">IF(C68=C67,1,0)</f>
+        <f t="shared" ref="S68:S69" si="24">IF(C68=C67,1,0)</f>
         <v>1</v>
       </c>
       <c r="T68" s="4">
-        <f t="shared" ref="T68:T69" si="14">IF(C68=C69,1,0)</f>
+        <f t="shared" ref="T68:T69" si="25">IF(C68=C69,1,0)</f>
         <v>1</v>
       </c>
       <c r="U68" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="B69" t="s">
@@ -7139,19 +7140,19 @@
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
       <c r="J69" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>44866</v>
       </c>
       <c r="K69" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>44895</v>
       </c>
       <c r="L69" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="21"/>
         <v>0 - MCE - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="M69" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>0 - MCR - 202211 - 30000000000 - Cliente</v>
       </c>
       <c r="N69" s="5" t="str">
@@ -7163,27 +7164,27 @@
         <v>#N/A</v>
       </c>
       <c r="P69" s="5" t="e">
-        <f>IF(EXACT(O69,E69),"ü","x")</f>
+        <f t="shared" si="17"/>
         <v>#N/A</v>
       </c>
       <c r="Q69" s="4">
-        <f>ROW(A69)</f>
+        <f t="shared" si="13"/>
         <v>69</v>
       </c>
-      <c r="R69" s="4" t="str">
-        <f>TEXT(J69,"AAAAMM")</f>
+      <c r="R69" s="2" t="str">
+        <f t="shared" si="23"/>
         <v>202211</v>
       </c>
       <c r="S69" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="T69" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="U69" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>